<commit_message>
Updated Iteration one log
</commit_message>
<xml_diff>
--- a/Initial Planning/Timeline.xlsx
+++ b/Initial Planning/Timeline.xlsx
@@ -334,9 +334,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" textRotation="180"/>
     </xf>
@@ -376,6 +373,9 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -695,8 +695,8 @@
   </sheetPr>
   <dimension ref="A1:DM225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH30" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="30" workbookViewId="0">
-      <selection sqref="A1:CU44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="30" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,323 +768,323 @@
     <col min="118" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:117" s="29" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:117" s="28" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="26">
+      <c r="B1" s="25">
         <v>1</v>
       </c>
-      <c r="C1" s="26">
+      <c r="C1" s="25">
         <v>2</v>
       </c>
-      <c r="D1" s="26">
+      <c r="D1" s="25">
         <v>3</v>
       </c>
-      <c r="E1" s="26">
+      <c r="E1" s="25">
         <v>4</v>
       </c>
-      <c r="F1" s="26">
+      <c r="F1" s="25">
         <v>5</v>
       </c>
-      <c r="G1" s="27">
+      <c r="G1" s="26">
         <v>6</v>
       </c>
-      <c r="H1" s="28">
+      <c r="H1" s="27">
         <v>7</v>
       </c>
-      <c r="I1" s="29">
+      <c r="I1" s="28">
         <v>8</v>
       </c>
-      <c r="J1" s="29">
+      <c r="J1" s="28">
         <v>9</v>
       </c>
-      <c r="K1" s="27">
+      <c r="K1" s="26">
         <v>10</v>
       </c>
-      <c r="L1" s="28">
+      <c r="L1" s="27">
         <v>11</v>
       </c>
-      <c r="M1" s="29">
+      <c r="M1" s="28">
         <v>12</v>
       </c>
-      <c r="N1" s="29">
+      <c r="N1" s="28">
         <v>13</v>
       </c>
-      <c r="O1" s="27">
+      <c r="O1" s="26">
         <v>14</v>
       </c>
-      <c r="P1" s="28">
+      <c r="P1" s="27">
         <v>15</v>
       </c>
-      <c r="Q1" s="29">
+      <c r="Q1" s="28">
         <v>16</v>
       </c>
-      <c r="R1" s="29">
+      <c r="R1" s="28">
         <v>17</v>
       </c>
-      <c r="S1" s="30">
+      <c r="S1" s="29">
         <v>18</v>
       </c>
-      <c r="T1" s="28">
+      <c r="T1" s="27">
         <v>19</v>
       </c>
-      <c r="U1" s="28">
+      <c r="U1" s="27">
         <v>20</v>
       </c>
-      <c r="V1" s="29">
+      <c r="V1" s="28">
         <v>21</v>
       </c>
-      <c r="W1" s="29">
+      <c r="W1" s="28">
         <v>22</v>
       </c>
-      <c r="X1" s="28">
+      <c r="X1" s="27">
         <v>23</v>
       </c>
-      <c r="Y1" s="28">
+      <c r="Y1" s="27">
         <v>24</v>
       </c>
-      <c r="Z1" s="29">
+      <c r="Z1" s="28">
         <v>25</v>
       </c>
-      <c r="AA1" s="29">
+      <c r="AA1" s="28">
         <v>26</v>
       </c>
-      <c r="AB1" s="28">
+      <c r="AB1" s="27">
         <v>27</v>
       </c>
-      <c r="AC1" s="28">
+      <c r="AC1" s="27">
         <v>28</v>
       </c>
-      <c r="AD1" s="29">
+      <c r="AD1" s="28">
         <v>29</v>
       </c>
-      <c r="AE1" s="29">
+      <c r="AE1" s="28">
         <v>30</v>
       </c>
-      <c r="AF1" s="30">
+      <c r="AF1" s="29">
         <v>31</v>
       </c>
-      <c r="AG1" s="28">
+      <c r="AG1" s="27">
         <v>32</v>
       </c>
-      <c r="AH1" s="28">
+      <c r="AH1" s="27">
         <v>33</v>
       </c>
-      <c r="AI1" s="29">
+      <c r="AI1" s="28">
         <v>34</v>
       </c>
-      <c r="AJ1" s="29">
+      <c r="AJ1" s="28">
         <v>35</v>
       </c>
-      <c r="AK1" s="28">
+      <c r="AK1" s="27">
         <v>36</v>
       </c>
-      <c r="AL1" s="28">
+      <c r="AL1" s="27">
         <v>37</v>
       </c>
-      <c r="AM1" s="29">
+      <c r="AM1" s="28">
         <v>38</v>
       </c>
-      <c r="AN1" s="29">
+      <c r="AN1" s="28">
         <v>39</v>
       </c>
-      <c r="AO1" s="28">
+      <c r="AO1" s="27">
         <v>40</v>
       </c>
-      <c r="AP1" s="28">
+      <c r="AP1" s="27">
         <v>41</v>
       </c>
-      <c r="AQ1" s="29">
+      <c r="AQ1" s="28">
         <v>42</v>
       </c>
-      <c r="AR1" s="29">
+      <c r="AR1" s="28">
         <v>43</v>
       </c>
-      <c r="AS1" s="28">
+      <c r="AS1" s="27">
         <v>44</v>
       </c>
-      <c r="AT1" s="28">
+      <c r="AT1" s="27">
         <v>45</v>
       </c>
-      <c r="AU1" s="29">
+      <c r="AU1" s="28">
         <v>46</v>
       </c>
-      <c r="AV1" s="29">
+      <c r="AV1" s="28">
         <v>47</v>
       </c>
-      <c r="AW1" s="28">
+      <c r="AW1" s="27">
         <v>48</v>
       </c>
-      <c r="AX1" s="28">
+      <c r="AX1" s="27">
         <v>49</v>
       </c>
-      <c r="AY1" s="29">
+      <c r="AY1" s="28">
         <v>50</v>
       </c>
-      <c r="AZ1" s="29">
+      <c r="AZ1" s="28">
         <v>51</v>
       </c>
-      <c r="BA1" s="28">
+      <c r="BA1" s="27">
         <v>52</v>
       </c>
-      <c r="BB1" s="28">
+      <c r="BB1" s="27">
         <v>53</v>
       </c>
-      <c r="BC1" s="29">
+      <c r="BC1" s="28">
         <v>54</v>
       </c>
-      <c r="BD1" s="29">
+      <c r="BD1" s="28">
         <v>55</v>
       </c>
-      <c r="BE1" s="30">
+      <c r="BE1" s="29">
         <v>56</v>
       </c>
-      <c r="BF1" s="28">
+      <c r="BF1" s="27">
         <v>57</v>
       </c>
-      <c r="BG1" s="28">
+      <c r="BG1" s="27">
         <v>58</v>
       </c>
-      <c r="BH1" s="29">
+      <c r="BH1" s="28">
         <v>59</v>
       </c>
-      <c r="BI1" s="29">
+      <c r="BI1" s="28">
         <v>60</v>
       </c>
-      <c r="BJ1" s="28">
+      <c r="BJ1" s="27">
         <v>61</v>
       </c>
-      <c r="BK1" s="28">
+      <c r="BK1" s="27">
         <v>62</v>
       </c>
-      <c r="BL1" s="29">
+      <c r="BL1" s="28">
         <v>63</v>
       </c>
-      <c r="BM1" s="29">
+      <c r="BM1" s="28">
         <v>64</v>
       </c>
-      <c r="BN1" s="28">
+      <c r="BN1" s="27">
         <v>65</v>
       </c>
-      <c r="BO1" s="28">
+      <c r="BO1" s="27">
         <v>66</v>
       </c>
-      <c r="BP1" s="29">
+      <c r="BP1" s="28">
         <v>67</v>
       </c>
-      <c r="BQ1" s="29">
+      <c r="BQ1" s="28">
         <v>68</v>
       </c>
-      <c r="BR1" s="28">
+      <c r="BR1" s="27">
         <v>69</v>
       </c>
-      <c r="BS1" s="28">
+      <c r="BS1" s="27">
         <v>70</v>
       </c>
-      <c r="BT1" s="29">
+      <c r="BT1" s="28">
         <v>71</v>
       </c>
-      <c r="BU1" s="29">
+      <c r="BU1" s="28">
         <v>72</v>
       </c>
-      <c r="BV1" s="27">
+      <c r="BV1" s="26">
         <v>73</v>
       </c>
-      <c r="BW1" s="27">
+      <c r="BW1" s="26">
         <v>74</v>
       </c>
-      <c r="BX1" s="29">
+      <c r="BX1" s="28">
         <v>75</v>
       </c>
-      <c r="BY1" s="29">
+      <c r="BY1" s="28">
         <v>76</v>
       </c>
-      <c r="BZ1" s="30">
+      <c r="BZ1" s="29">
         <v>77</v>
       </c>
-      <c r="CA1" s="27">
+      <c r="CA1" s="26">
         <v>78</v>
       </c>
-      <c r="CB1" s="28">
+      <c r="CB1" s="27">
         <v>79</v>
       </c>
-      <c r="CC1" s="29">
+      <c r="CC1" s="28">
         <v>80</v>
       </c>
-      <c r="CD1" s="29">
+      <c r="CD1" s="28">
         <v>81</v>
       </c>
-      <c r="CE1" s="27">
+      <c r="CE1" s="26">
         <v>82</v>
       </c>
-      <c r="CF1" s="28">
+      <c r="CF1" s="27">
         <v>83</v>
       </c>
-      <c r="CG1" s="29">
+      <c r="CG1" s="28">
         <v>84</v>
       </c>
-      <c r="CH1" s="29">
+      <c r="CH1" s="28">
         <v>85</v>
       </c>
-      <c r="CI1" s="27">
+      <c r="CI1" s="26">
         <v>86</v>
       </c>
-      <c r="CJ1" s="28">
+      <c r="CJ1" s="27">
         <v>87</v>
       </c>
-      <c r="CK1" s="29">
+      <c r="CK1" s="28">
         <v>88</v>
       </c>
-      <c r="CL1" s="29">
+      <c r="CL1" s="28">
         <v>89</v>
       </c>
-      <c r="CM1" s="27">
+      <c r="CM1" s="26">
         <v>90</v>
       </c>
-      <c r="CN1" s="28">
+      <c r="CN1" s="27">
         <v>91</v>
       </c>
-      <c r="CO1" s="30">
+      <c r="CO1" s="29">
         <v>92</v>
       </c>
-      <c r="CP1" s="26">
+      <c r="CP1" s="25">
         <v>93</v>
       </c>
-      <c r="CQ1" s="26">
+      <c r="CQ1" s="25">
         <v>94</v>
       </c>
-      <c r="CR1" s="26">
+      <c r="CR1" s="25">
         <v>95</v>
       </c>
-      <c r="CS1" s="26">
+      <c r="CS1" s="25">
         <v>96</v>
       </c>
-      <c r="CT1" s="26">
+      <c r="CT1" s="25">
         <v>97</v>
       </c>
-      <c r="CU1" s="31">
+      <c r="CU1" s="30">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:117" s="12" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+    <row r="2" spans="1:117" s="11" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="S2" s="13" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="S2" s="12" t="s">
         <v>34</v>
       </c>
       <c r="T2" s="8"/>
@@ -1098,7 +1098,7 @@
       <c r="AC2" s="8"/>
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
-      <c r="AF2" s="13" t="s">
+      <c r="AF2" s="12" t="s">
         <v>34</v>
       </c>
       <c r="AG2" s="8"/>
@@ -1125,7 +1125,7 @@
       <c r="BB2" s="8"/>
       <c r="BC2" s="3"/>
       <c r="BD2" s="3"/>
-      <c r="BE2" s="13" t="s">
+      <c r="BE2" s="12" t="s">
         <v>34</v>
       </c>
       <c r="BF2" s="8"/>
@@ -1142,33 +1142,33 @@
       <c r="BS2" s="8"/>
       <c r="BT2" s="3"/>
       <c r="BV2" s="8"/>
-      <c r="BW2" s="11"/>
+      <c r="BW2" s="10"/>
       <c r="BX2" s="3"/>
-      <c r="BZ2" s="13" t="s">
+      <c r="BZ2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="CA2" s="11"/>
+      <c r="CA2" s="10"/>
       <c r="CB2" s="8"/>
       <c r="CD2" s="3"/>
-      <c r="CE2" s="11"/>
+      <c r="CE2" s="10"/>
       <c r="CF2" s="8"/>
       <c r="CH2" s="3"/>
-      <c r="CI2" s="11"/>
+      <c r="CI2" s="10"/>
       <c r="CJ2" s="8"/>
       <c r="CL2" s="3"/>
-      <c r="CM2" s="11"/>
+      <c r="CM2" s="10"/>
       <c r="CN2" s="8"/>
-      <c r="CO2" s="13" t="s">
+      <c r="CO2" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="CP2" s="10" t="s">
+      <c r="CP2" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="CQ2" s="10"/>
-      <c r="CR2" s="10"/>
-      <c r="CS2" s="10"/>
-      <c r="CT2" s="10"/>
-      <c r="CU2" s="14" t="s">
+      <c r="CQ2" s="32"/>
+      <c r="CR2" s="32"/>
+      <c r="CS2" s="32"/>
+      <c r="CT2" s="32"/>
+      <c r="CU2" s="13" t="s">
         <v>44</v>
       </c>
       <c r="CW2" s="3"/>
@@ -1194,19 +1194,19 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="9"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
       <c r="X3" s="8"/>
       <c r="Y3" s="8"/>
-      <c r="Z3" s="16"/>
+      <c r="Z3" s="15"/>
       <c r="AA3" s="3"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="8"/>
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
-      <c r="AF3" s="17"/>
+      <c r="AF3" s="16"/>
       <c r="AG3" s="8"/>
       <c r="AH3" s="8"/>
       <c r="AI3" s="3"/>
@@ -1231,7 +1231,7 @@
       <c r="BB3" s="8"/>
       <c r="BC3" s="3"/>
       <c r="BD3" s="3"/>
-      <c r="BE3" s="17"/>
+      <c r="BE3" s="16"/>
       <c r="BF3" s="8"/>
       <c r="BG3" s="8"/>
       <c r="BH3" s="3"/>
@@ -1308,17 +1308,17 @@
       <c r="S4" s="9"/>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
-      <c r="V4" s="15"/>
-      <c r="W4" s="15"/>
-      <c r="X4" s="15"/>
-      <c r="Y4" s="15"/>
-      <c r="Z4" s="15"/>
-      <c r="AA4" s="15"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="8"/>
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
-      <c r="AF4" s="17"/>
+      <c r="AF4" s="16"/>
       <c r="AG4" s="8"/>
       <c r="AH4" s="8"/>
       <c r="AI4" s="3"/>
@@ -1420,17 +1420,17 @@
       <c r="S5" s="9"/>
       <c r="T5" s="8"/>
       <c r="U5" s="8"/>
-      <c r="V5" s="15"/>
-      <c r="W5" s="15"/>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
       <c r="AB5" s="8"/>
       <c r="AC5" s="8"/>
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
-      <c r="AF5" s="17"/>
+      <c r="AF5" s="16"/>
       <c r="AG5" s="8"/>
       <c r="AH5" s="8"/>
       <c r="AI5" s="3"/>
@@ -1531,12 +1531,12 @@
       <c r="S6" s="9"/>
       <c r="T6" s="8"/>
       <c r="U6" s="8"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
-      <c r="Y6" s="15"/>
-      <c r="Z6" s="15"/>
-      <c r="AA6" s="15"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
+      <c r="Z6" s="14"/>
+      <c r="AA6" s="14"/>
       <c r="AB6" s="8"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="3"/>
@@ -1566,7 +1566,7 @@
       <c r="BB6" s="8"/>
       <c r="BC6" s="3"/>
       <c r="BD6" s="3"/>
-      <c r="BE6" s="17"/>
+      <c r="BE6" s="16"/>
       <c r="BF6" s="8"/>
       <c r="BG6" s="8"/>
       <c r="BH6" s="3"/>
@@ -1574,7 +1574,7 @@
       <c r="BJ6" s="8"/>
       <c r="BK6" s="8"/>
       <c r="BL6" s="3"/>
-      <c r="BM6" s="16"/>
+      <c r="BM6" s="15"/>
       <c r="BN6" s="8"/>
       <c r="BO6" s="8"/>
       <c r="BP6" s="3"/>
@@ -1635,10 +1635,10 @@
       <c r="J7" s="3"/>
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="15"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
       <c r="S7" s="9"/>
@@ -1679,7 +1679,7 @@
       <c r="BB7" s="8"/>
       <c r="BC7" s="3"/>
       <c r="BD7" s="3"/>
-      <c r="BE7" s="17"/>
+      <c r="BE7" s="16"/>
       <c r="BF7" s="8"/>
       <c r="BG7" s="8"/>
       <c r="BH7" s="3"/>
@@ -1687,11 +1687,11 @@
       <c r="BJ7" s="8"/>
       <c r="BK7" s="8"/>
       <c r="BL7" s="3"/>
-      <c r="BM7" s="16"/>
+      <c r="BM7" s="15"/>
       <c r="BN7" s="8"/>
       <c r="BO7" s="8"/>
       <c r="BP7" s="3"/>
-      <c r="BQ7" s="16"/>
+      <c r="BQ7" s="15"/>
       <c r="BR7" s="8"/>
       <c r="BS7" s="8"/>
       <c r="BT7" s="3"/>
@@ -1748,10 +1748,10 @@
       <c r="J8" s="3"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="9"/>
@@ -1800,23 +1800,23 @@
       <c r="BJ8" s="8"/>
       <c r="BK8" s="8"/>
       <c r="BL8" s="3"/>
-      <c r="BM8" s="16"/>
+      <c r="BM8" s="15"/>
       <c r="BN8" s="8"/>
       <c r="BO8" s="8"/>
       <c r="BP8" s="3"/>
-      <c r="BQ8" s="16"/>
+      <c r="BQ8" s="15"/>
       <c r="BR8" s="8"/>
       <c r="BS8" s="8"/>
       <c r="BT8" s="3"/>
-      <c r="BU8" s="16"/>
+      <c r="BU8" s="15"/>
       <c r="BV8" s="8"/>
-      <c r="BW8" s="18"/>
+      <c r="BW8" s="17"/>
       <c r="BX8" s="3"/>
-      <c r="BY8" s="16"/>
-      <c r="BZ8" s="17"/>
-      <c r="CA8" s="18"/>
+      <c r="BY8" s="15"/>
+      <c r="BZ8" s="16"/>
+      <c r="CA8" s="17"/>
       <c r="CB8" s="8"/>
-      <c r="CC8" s="16"/>
+      <c r="CC8" s="15"/>
       <c r="CD8" s="3"/>
       <c r="CF8" s="8"/>
       <c r="CG8" s="3"/>
@@ -1850,21 +1850,21 @@
       <c r="DL8" s="3"/>
       <c r="DM8" s="3"/>
     </row>
-    <row r="9" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="7"/>
@@ -1931,48 +1931,48 @@
       <c r="BX9" s="3"/>
       <c r="BY9" s="3"/>
       <c r="BZ9" s="9"/>
-      <c r="CA9" s="18"/>
+      <c r="CA9" s="17"/>
       <c r="CB9" s="8"/>
-      <c r="CC9" s="16"/>
+      <c r="CC9" s="15"/>
       <c r="CD9" s="3"/>
-      <c r="CE9" s="18"/>
+      <c r="CE9" s="17"/>
       <c r="CF9" s="8"/>
-      <c r="CG9" s="16"/>
+      <c r="CG9" s="15"/>
       <c r="CH9" s="3"/>
-      <c r="CI9" s="18"/>
+      <c r="CI9" s="17"/>
       <c r="CJ9" s="8"/>
-      <c r="CK9" s="16"/>
+      <c r="CK9" s="15"/>
       <c r="CL9" s="3"/>
-      <c r="CM9" s="18"/>
+      <c r="CM9" s="17"/>
       <c r="CN9" s="8"/>
-      <c r="CO9" s="17"/>
-      <c r="CP9" s="20"/>
+      <c r="CO9" s="16"/>
+      <c r="CP9" s="19"/>
       <c r="CQ9" s="6"/>
       <c r="CR9" s="6"/>
       <c r="CS9" s="6"/>
       <c r="CT9" s="6"/>
-      <c r="CU9" s="21"/>
+      <c r="CU9" s="20"/>
       <c r="CX9" s="3"/>
       <c r="CY9" s="3"/>
       <c r="CZ9" s="3"/>
       <c r="DA9" s="3"/>
       <c r="DB9" s="3"/>
     </row>
-    <row r="10" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="7"/>
@@ -2051,34 +2051,34 @@
       <c r="CJ10" s="8"/>
       <c r="CK10" s="3"/>
       <c r="CL10" s="3"/>
-      <c r="CM10" s="18"/>
+      <c r="CM10" s="17"/>
       <c r="CN10" s="8"/>
-      <c r="CO10" s="17"/>
-      <c r="CP10" s="20"/>
-      <c r="CQ10" s="20"/>
-      <c r="CR10" s="20"/>
-      <c r="CS10" s="20"/>
-      <c r="CT10" s="20"/>
-      <c r="CU10" s="21"/>
-      <c r="CX10" s="16"/>
+      <c r="CO10" s="16"/>
+      <c r="CP10" s="19"/>
+      <c r="CQ10" s="19"/>
+      <c r="CR10" s="19"/>
+      <c r="CS10" s="19"/>
+      <c r="CT10" s="19"/>
+      <c r="CU10" s="20"/>
+      <c r="CX10" s="15"/>
       <c r="CY10" s="3"/>
       <c r="CZ10" s="3"/>
       <c r="DA10" s="3"/>
       <c r="DB10" s="3"/>
     </row>
-    <row r="11" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
       <c r="M11" s="3"/>
@@ -2159,30 +2159,30 @@
       <c r="CJ11" s="8"/>
       <c r="CK11" s="3"/>
       <c r="CL11" s="3"/>
-      <c r="CM11" s="18"/>
+      <c r="CM11" s="17"/>
       <c r="CN11" s="8"/>
-      <c r="CO11" s="17"/>
-      <c r="CP11" s="20"/>
-      <c r="CQ11" s="20"/>
-      <c r="CR11" s="20"/>
-      <c r="CS11" s="20"/>
-      <c r="CT11" s="20"/>
-      <c r="CU11" s="21"/>
-      <c r="CX11" s="16"/>
+      <c r="CO11" s="16"/>
+      <c r="CP11" s="19"/>
+      <c r="CQ11" s="19"/>
+      <c r="CR11" s="19"/>
+      <c r="CS11" s="19"/>
+      <c r="CT11" s="19"/>
+      <c r="CU11" s="20"/>
+      <c r="CX11" s="15"/>
       <c r="CY11" s="3"/>
       <c r="CZ11" s="3"/>
       <c r="DA11" s="3"/>
       <c r="DB11" s="3"/>
     </row>
-    <row r="12" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="3"/>
@@ -2193,8 +2193,8 @@
       <c r="N12" s="3"/>
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
       <c r="S12" s="9"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8"/>
@@ -2267,30 +2267,30 @@
       <c r="CJ12" s="8"/>
       <c r="CK12" s="3"/>
       <c r="CL12" s="3"/>
-      <c r="CM12" s="18"/>
+      <c r="CM12" s="17"/>
       <c r="CN12" s="8"/>
-      <c r="CO12" s="17"/>
-      <c r="CP12" s="20"/>
-      <c r="CQ12" s="20"/>
-      <c r="CR12" s="20"/>
-      <c r="CS12" s="20"/>
-      <c r="CT12" s="20"/>
-      <c r="CU12" s="21"/>
-      <c r="CX12" s="16"/>
+      <c r="CO12" s="16"/>
+      <c r="CP12" s="19"/>
+      <c r="CQ12" s="19"/>
+      <c r="CR12" s="19"/>
+      <c r="CS12" s="19"/>
+      <c r="CT12" s="19"/>
+      <c r="CU12" s="20"/>
+      <c r="CX12" s="15"/>
       <c r="CY12" s="3"/>
       <c r="CZ12" s="3"/>
       <c r="DA12" s="3"/>
       <c r="DB12" s="3"/>
     </row>
-    <row r="13" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="3"/>
@@ -2346,10 +2346,10 @@
       <c r="BG13" s="8"/>
       <c r="BH13" s="3"/>
       <c r="BI13" s="3"/>
-      <c r="BJ13" s="15"/>
-      <c r="BK13" s="15"/>
-      <c r="BL13" s="15"/>
-      <c r="BM13" s="15"/>
+      <c r="BJ13" s="14"/>
+      <c r="BK13" s="14"/>
+      <c r="BL13" s="14"/>
+      <c r="BM13" s="14"/>
       <c r="BN13" s="8"/>
       <c r="BO13" s="8"/>
       <c r="BP13" s="3"/>
@@ -2375,30 +2375,30 @@
       <c r="CJ13" s="8"/>
       <c r="CK13" s="3"/>
       <c r="CL13" s="3"/>
-      <c r="CM13" s="18"/>
+      <c r="CM13" s="17"/>
       <c r="CN13" s="8"/>
-      <c r="CO13" s="17"/>
-      <c r="CP13" s="20"/>
-      <c r="CQ13" s="20"/>
-      <c r="CR13" s="20"/>
-      <c r="CS13" s="20"/>
-      <c r="CT13" s="20"/>
-      <c r="CU13" s="21"/>
-      <c r="CX13" s="16"/>
+      <c r="CO13" s="16"/>
+      <c r="CP13" s="19"/>
+      <c r="CQ13" s="19"/>
+      <c r="CR13" s="19"/>
+      <c r="CS13" s="19"/>
+      <c r="CT13" s="19"/>
+      <c r="CU13" s="20"/>
+      <c r="CX13" s="15"/>
       <c r="CY13" s="3"/>
       <c r="CZ13" s="3"/>
       <c r="DA13" s="3"/>
       <c r="DB13" s="3"/>
     </row>
-    <row r="14" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="3"/>
@@ -2412,10 +2412,10 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="3"/>
@@ -2483,30 +2483,30 @@
       <c r="CJ14" s="8"/>
       <c r="CK14" s="3"/>
       <c r="CL14" s="3"/>
-      <c r="CM14" s="18"/>
+      <c r="CM14" s="17"/>
       <c r="CN14" s="8"/>
-      <c r="CO14" s="17"/>
-      <c r="CP14" s="20"/>
-      <c r="CQ14" s="20"/>
-      <c r="CR14" s="20"/>
-      <c r="CS14" s="20"/>
-      <c r="CT14" s="20"/>
-      <c r="CU14" s="21"/>
-      <c r="CX14" s="16"/>
+      <c r="CO14" s="16"/>
+      <c r="CP14" s="19"/>
+      <c r="CQ14" s="19"/>
+      <c r="CR14" s="19"/>
+      <c r="CS14" s="19"/>
+      <c r="CT14" s="19"/>
+      <c r="CU14" s="20"/>
+      <c r="CX14" s="15"/>
       <c r="CY14" s="3"/>
       <c r="CZ14" s="3"/>
       <c r="DA14" s="3"/>
       <c r="DB14" s="3"/>
     </row>
-    <row r="15" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="3"/>
@@ -2526,10 +2526,10 @@
       <c r="W15" s="3"/>
       <c r="X15" s="8"/>
       <c r="Y15" s="8"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
+      <c r="Z15" s="14"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="14"/>
+      <c r="AC15" s="14"/>
       <c r="AD15" s="3"/>
       <c r="AE15" s="3"/>
       <c r="AF15" s="9"/>
@@ -2591,30 +2591,30 @@
       <c r="CJ15" s="8"/>
       <c r="CK15" s="3"/>
       <c r="CL15" s="3"/>
-      <c r="CM15" s="18"/>
+      <c r="CM15" s="17"/>
       <c r="CN15" s="8"/>
-      <c r="CO15" s="17"/>
-      <c r="CP15" s="20"/>
-      <c r="CQ15" s="20"/>
-      <c r="CR15" s="20"/>
-      <c r="CS15" s="20"/>
-      <c r="CT15" s="20"/>
-      <c r="CU15" s="21"/>
-      <c r="CX15" s="16"/>
+      <c r="CO15" s="16"/>
+      <c r="CP15" s="19"/>
+      <c r="CQ15" s="19"/>
+      <c r="CR15" s="19"/>
+      <c r="CS15" s="19"/>
+      <c r="CT15" s="19"/>
+      <c r="CU15" s="20"/>
+      <c r="CX15" s="15"/>
       <c r="CY15" s="3"/>
       <c r="CZ15" s="3"/>
       <c r="DA15" s="3"/>
       <c r="DB15" s="3"/>
     </row>
-    <row r="16" spans="1:117" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:117" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
       <c r="I16" s="3"/>
@@ -2645,16 +2645,16 @@
       <c r="AH16" s="8"/>
       <c r="AI16" s="3"/>
       <c r="AJ16" s="3"/>
-      <c r="AK16" s="15"/>
-      <c r="AL16" s="15"/>
-      <c r="AM16" s="15"/>
-      <c r="AN16" s="15"/>
-      <c r="AO16" s="15"/>
-      <c r="AP16" s="15"/>
-      <c r="AQ16" s="15"/>
-      <c r="AR16" s="15"/>
-      <c r="AS16" s="15"/>
-      <c r="AT16" s="15"/>
+      <c r="AK16" s="14"/>
+      <c r="AL16" s="14"/>
+      <c r="AM16" s="14"/>
+      <c r="AN16" s="14"/>
+      <c r="AO16" s="14"/>
+      <c r="AP16" s="14"/>
+      <c r="AQ16" s="14"/>
+      <c r="AR16" s="14"/>
+      <c r="AS16" s="14"/>
+      <c r="AT16" s="14"/>
       <c r="AU16" s="3"/>
       <c r="AV16" s="3"/>
       <c r="AW16" s="8"/>
@@ -2699,30 +2699,30 @@
       <c r="CJ16" s="8"/>
       <c r="CK16" s="3"/>
       <c r="CL16" s="3"/>
-      <c r="CM16" s="18"/>
+      <c r="CM16" s="17"/>
       <c r="CN16" s="8"/>
-      <c r="CO16" s="17"/>
-      <c r="CP16" s="20"/>
-      <c r="CQ16" s="20"/>
-      <c r="CR16" s="20"/>
-      <c r="CS16" s="20"/>
-      <c r="CT16" s="20"/>
-      <c r="CU16" s="21"/>
-      <c r="CX16" s="16"/>
+      <c r="CO16" s="16"/>
+      <c r="CP16" s="19"/>
+      <c r="CQ16" s="19"/>
+      <c r="CR16" s="19"/>
+      <c r="CS16" s="19"/>
+      <c r="CT16" s="19"/>
+      <c r="CU16" s="20"/>
+      <c r="CX16" s="15"/>
       <c r="CY16" s="3"/>
       <c r="CZ16" s="3"/>
       <c r="DA16" s="3"/>
       <c r="DB16" s="3"/>
     </row>
-    <row r="17" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="3"/>
@@ -2749,12 +2749,12 @@
       <c r="AD17" s="3"/>
       <c r="AE17" s="3"/>
       <c r="AF17" s="9"/>
-      <c r="AG17" s="15"/>
-      <c r="AH17" s="15"/>
-      <c r="AI17" s="15"/>
-      <c r="AJ17" s="15"/>
-      <c r="AK17" s="15"/>
-      <c r="AL17" s="15"/>
+      <c r="AG17" s="14"/>
+      <c r="AH17" s="14"/>
+      <c r="AI17" s="14"/>
+      <c r="AJ17" s="14"/>
+      <c r="AK17" s="14"/>
+      <c r="AL17" s="14"/>
       <c r="AM17" s="3"/>
       <c r="AN17" s="3"/>
       <c r="AO17" s="8"/>
@@ -2807,30 +2807,30 @@
       <c r="CJ17" s="8"/>
       <c r="CK17" s="3"/>
       <c r="CL17" s="3"/>
-      <c r="CM17" s="18"/>
+      <c r="CM17" s="17"/>
       <c r="CN17" s="8"/>
-      <c r="CO17" s="17"/>
-      <c r="CP17" s="20"/>
-      <c r="CQ17" s="20"/>
-      <c r="CR17" s="20"/>
-      <c r="CS17" s="20"/>
-      <c r="CT17" s="20"/>
-      <c r="CU17" s="21"/>
-      <c r="CX17" s="16"/>
+      <c r="CO17" s="16"/>
+      <c r="CP17" s="19"/>
+      <c r="CQ17" s="19"/>
+      <c r="CR17" s="19"/>
+      <c r="CS17" s="19"/>
+      <c r="CT17" s="19"/>
+      <c r="CU17" s="20"/>
+      <c r="CX17" s="15"/>
       <c r="CY17" s="3"/>
       <c r="CZ17" s="3"/>
       <c r="DA17" s="3"/>
       <c r="DB17" s="3"/>
     </row>
-    <row r="18" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
       <c r="I18" s="3"/>
@@ -2861,8 +2861,8 @@
       <c r="AH18" s="8"/>
       <c r="AI18" s="3"/>
       <c r="AJ18" s="3"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
+      <c r="AK18" s="14"/>
+      <c r="AL18" s="14"/>
       <c r="AM18" s="3"/>
       <c r="AN18" s="3"/>
       <c r="AO18" s="8"/>
@@ -2915,30 +2915,30 @@
       <c r="CJ18" s="8"/>
       <c r="CK18" s="3"/>
       <c r="CL18" s="3"/>
-      <c r="CM18" s="18"/>
+      <c r="CM18" s="17"/>
       <c r="CN18" s="8"/>
-      <c r="CO18" s="17"/>
-      <c r="CP18" s="20"/>
-      <c r="CQ18" s="20"/>
-      <c r="CR18" s="20"/>
-      <c r="CS18" s="20"/>
-      <c r="CT18" s="20"/>
-      <c r="CU18" s="21"/>
-      <c r="CX18" s="16"/>
+      <c r="CO18" s="16"/>
+      <c r="CP18" s="19"/>
+      <c r="CQ18" s="19"/>
+      <c r="CR18" s="19"/>
+      <c r="CS18" s="19"/>
+      <c r="CT18" s="19"/>
+      <c r="CU18" s="20"/>
+      <c r="CX18" s="15"/>
       <c r="CY18" s="3"/>
       <c r="CZ18" s="3"/>
       <c r="DA18" s="3"/>
       <c r="DB18" s="3"/>
     </row>
-    <row r="19" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
       <c r="I19" s="3"/>
@@ -2971,8 +2971,8 @@
       <c r="AJ19" s="3"/>
       <c r="AK19" s="8"/>
       <c r="AL19" s="8"/>
-      <c r="AM19" s="15"/>
-      <c r="AN19" s="15"/>
+      <c r="AM19" s="14"/>
+      <c r="AN19" s="14"/>
       <c r="AO19" s="8"/>
       <c r="AP19" s="8"/>
       <c r="AQ19" s="3"/>
@@ -3023,30 +3023,30 @@
       <c r="CJ19" s="8"/>
       <c r="CK19" s="3"/>
       <c r="CL19" s="3"/>
-      <c r="CM19" s="18"/>
+      <c r="CM19" s="17"/>
       <c r="CN19" s="8"/>
-      <c r="CO19" s="17"/>
-      <c r="CP19" s="20"/>
-      <c r="CQ19" s="20"/>
-      <c r="CR19" s="20"/>
-      <c r="CS19" s="20"/>
-      <c r="CT19" s="20"/>
-      <c r="CU19" s="21"/>
-      <c r="CX19" s="16"/>
+      <c r="CO19" s="16"/>
+      <c r="CP19" s="19"/>
+      <c r="CQ19" s="19"/>
+      <c r="CR19" s="19"/>
+      <c r="CS19" s="19"/>
+      <c r="CT19" s="19"/>
+      <c r="CU19" s="20"/>
+      <c r="CX19" s="15"/>
       <c r="CY19" s="3"/>
       <c r="CZ19" s="3"/>
       <c r="DA19" s="3"/>
       <c r="DB19" s="3"/>
     </row>
-    <row r="20" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
       <c r="I20" s="3"/>
@@ -3131,30 +3131,30 @@
       <c r="CJ20" s="8"/>
       <c r="CK20" s="3"/>
       <c r="CL20" s="3"/>
-      <c r="CM20" s="18"/>
+      <c r="CM20" s="17"/>
       <c r="CN20" s="8"/>
-      <c r="CO20" s="17"/>
-      <c r="CP20" s="20"/>
-      <c r="CQ20" s="20"/>
-      <c r="CR20" s="20"/>
-      <c r="CS20" s="20"/>
-      <c r="CT20" s="20"/>
-      <c r="CU20" s="21"/>
-      <c r="CX20" s="16"/>
+      <c r="CO20" s="16"/>
+      <c r="CP20" s="19"/>
+      <c r="CQ20" s="19"/>
+      <c r="CR20" s="19"/>
+      <c r="CS20" s="19"/>
+      <c r="CT20" s="19"/>
+      <c r="CU20" s="20"/>
+      <c r="CX20" s="15"/>
       <c r="CY20" s="3"/>
       <c r="CZ20" s="3"/>
       <c r="DA20" s="3"/>
       <c r="DB20" s="3"/>
     </row>
-    <row r="21" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
       <c r="I21" s="3"/>
@@ -3214,14 +3214,14 @@
       <c r="BK21" s="8"/>
       <c r="BL21" s="3"/>
       <c r="BM21" s="3"/>
-      <c r="BN21" s="15"/>
-      <c r="BO21" s="15"/>
-      <c r="BP21" s="15"/>
-      <c r="BQ21" s="15"/>
-      <c r="BR21" s="15"/>
-      <c r="BS21" s="15"/>
-      <c r="BT21" s="15"/>
-      <c r="BU21" s="15"/>
+      <c r="BN21" s="14"/>
+      <c r="BO21" s="14"/>
+      <c r="BP21" s="14"/>
+      <c r="BQ21" s="14"/>
+      <c r="BR21" s="14"/>
+      <c r="BS21" s="14"/>
+      <c r="BT21" s="14"/>
+      <c r="BU21" s="14"/>
       <c r="BV21" s="8"/>
       <c r="BW21" s="7"/>
       <c r="BX21" s="3"/>
@@ -3239,30 +3239,30 @@
       <c r="CJ21" s="8"/>
       <c r="CK21" s="3"/>
       <c r="CL21" s="3"/>
-      <c r="CM21" s="18"/>
+      <c r="CM21" s="17"/>
       <c r="CN21" s="8"/>
-      <c r="CO21" s="17"/>
-      <c r="CP21" s="20"/>
-      <c r="CQ21" s="20"/>
-      <c r="CR21" s="20"/>
-      <c r="CS21" s="20"/>
-      <c r="CT21" s="20"/>
-      <c r="CU21" s="21"/>
-      <c r="CX21" s="16"/>
+      <c r="CO21" s="16"/>
+      <c r="CP21" s="19"/>
+      <c r="CQ21" s="19"/>
+      <c r="CR21" s="19"/>
+      <c r="CS21" s="19"/>
+      <c r="CT21" s="19"/>
+      <c r="CU21" s="20"/>
+      <c r="CX21" s="15"/>
       <c r="CY21" s="3"/>
       <c r="CZ21" s="3"/>
       <c r="DA21" s="3"/>
       <c r="DB21" s="3"/>
     </row>
-    <row r="22" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="3"/>
@@ -3297,8 +3297,8 @@
       <c r="AL22" s="8"/>
       <c r="AM22" s="3"/>
       <c r="AN22" s="3"/>
-      <c r="AO22" s="15"/>
-      <c r="AP22" s="15"/>
+      <c r="AO22" s="14"/>
+      <c r="AP22" s="14"/>
       <c r="AQ22" s="3"/>
       <c r="AR22" s="3"/>
       <c r="AS22" s="8"/>
@@ -3347,30 +3347,30 @@
       <c r="CJ22" s="8"/>
       <c r="CK22" s="3"/>
       <c r="CL22" s="3"/>
-      <c r="CM22" s="18"/>
+      <c r="CM22" s="17"/>
       <c r="CN22" s="8"/>
-      <c r="CO22" s="17"/>
-      <c r="CP22" s="20"/>
-      <c r="CQ22" s="20"/>
-      <c r="CR22" s="20"/>
-      <c r="CS22" s="20"/>
-      <c r="CT22" s="20"/>
-      <c r="CU22" s="21"/>
-      <c r="CX22" s="16"/>
+      <c r="CO22" s="16"/>
+      <c r="CP22" s="19"/>
+      <c r="CQ22" s="19"/>
+      <c r="CR22" s="19"/>
+      <c r="CS22" s="19"/>
+      <c r="CT22" s="19"/>
+      <c r="CU22" s="20"/>
+      <c r="CX22" s="15"/>
       <c r="CY22" s="3"/>
       <c r="CZ22" s="3"/>
       <c r="DA22" s="3"/>
       <c r="DB22" s="3"/>
     </row>
-    <row r="23" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="3"/>
@@ -3451,34 +3451,34 @@
       <c r="CF23" s="8"/>
       <c r="CG23" s="3"/>
       <c r="CH23" s="3"/>
-      <c r="CI23" s="15"/>
-      <c r="CJ23" s="15"/>
+      <c r="CI23" s="14"/>
+      <c r="CJ23" s="14"/>
       <c r="CK23" s="3"/>
       <c r="CL23" s="3"/>
-      <c r="CM23" s="15"/>
-      <c r="CN23" s="15"/>
-      <c r="CO23" s="17"/>
-      <c r="CP23" s="20"/>
-      <c r="CQ23" s="20"/>
-      <c r="CR23" s="20"/>
-      <c r="CS23" s="20"/>
-      <c r="CT23" s="20"/>
-      <c r="CU23" s="21"/>
-      <c r="CX23" s="16"/>
+      <c r="CM23" s="14"/>
+      <c r="CN23" s="14"/>
+      <c r="CO23" s="16"/>
+      <c r="CP23" s="19"/>
+      <c r="CQ23" s="19"/>
+      <c r="CR23" s="19"/>
+      <c r="CS23" s="19"/>
+      <c r="CT23" s="19"/>
+      <c r="CU23" s="20"/>
+      <c r="CX23" s="15"/>
       <c r="CY23" s="3"/>
       <c r="CZ23" s="3"/>
       <c r="DA23" s="3"/>
       <c r="DB23" s="3"/>
     </row>
-    <row r="24" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
       <c r="I24" s="3"/>
@@ -3502,8 +3502,8 @@
       <c r="AA24" s="3"/>
       <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="14"/>
       <c r="AF24" s="9"/>
       <c r="AG24" s="8"/>
       <c r="AH24" s="8"/>
@@ -3563,31 +3563,31 @@
       <c r="CJ24" s="8"/>
       <c r="CK24" s="3"/>
       <c r="CL24" s="3"/>
-      <c r="CM24" s="18"/>
+      <c r="CM24" s="17"/>
       <c r="CN24" s="8"/>
-      <c r="CO24" s="17"/>
-      <c r="CP24" s="20"/>
-      <c r="CQ24" s="20"/>
-      <c r="CR24" s="20"/>
-      <c r="CS24" s="20"/>
-      <c r="CT24" s="20"/>
-      <c r="CU24" s="21"/>
-      <c r="CX24" s="16"/>
+      <c r="CO24" s="16"/>
+      <c r="CP24" s="19"/>
+      <c r="CQ24" s="19"/>
+      <c r="CR24" s="19"/>
+      <c r="CS24" s="19"/>
+      <c r="CT24" s="19"/>
+      <c r="CU24" s="20"/>
+      <c r="CX24" s="15"/>
       <c r="CY24" s="3"/>
       <c r="CZ24" s="3"/>
       <c r="DA24" s="3"/>
       <c r="DB24" s="3"/>
       <c r="DC24" s="5"/>
     </row>
-    <row r="25" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
       <c r="I25" s="3"/>
@@ -3611,8 +3611,8 @@
       <c r="AA25" s="3"/>
       <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
-      <c r="AD25" s="15"/>
-      <c r="AE25" s="15"/>
+      <c r="AD25" s="14"/>
+      <c r="AE25" s="14"/>
       <c r="AF25" s="9"/>
       <c r="AG25" s="8"/>
       <c r="AH25" s="8"/>
@@ -3672,31 +3672,31 @@
       <c r="CJ25" s="8"/>
       <c r="CK25" s="3"/>
       <c r="CL25" s="3"/>
-      <c r="CM25" s="18"/>
+      <c r="CM25" s="17"/>
       <c r="CN25" s="8"/>
-      <c r="CO25" s="17"/>
-      <c r="CP25" s="20"/>
-      <c r="CQ25" s="20"/>
-      <c r="CR25" s="20"/>
-      <c r="CS25" s="20"/>
-      <c r="CT25" s="20"/>
-      <c r="CU25" s="21"/>
-      <c r="CX25" s="16"/>
+      <c r="CO25" s="16"/>
+      <c r="CP25" s="19"/>
+      <c r="CQ25" s="19"/>
+      <c r="CR25" s="19"/>
+      <c r="CS25" s="19"/>
+      <c r="CT25" s="19"/>
+      <c r="CU25" s="20"/>
+      <c r="CX25" s="15"/>
       <c r="CY25" s="3"/>
       <c r="CZ25" s="3"/>
       <c r="DA25" s="3"/>
       <c r="DB25" s="3"/>
       <c r="DC25" s="5"/>
     </row>
-    <row r="26" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
       <c r="I26" s="3"/>
@@ -3779,33 +3779,33 @@
       <c r="CH26" s="3"/>
       <c r="CI26" s="7"/>
       <c r="CJ26" s="8"/>
-      <c r="CK26" s="15"/>
-      <c r="CL26" s="15"/>
-      <c r="CM26" s="18"/>
+      <c r="CK26" s="14"/>
+      <c r="CL26" s="14"/>
+      <c r="CM26" s="17"/>
       <c r="CN26" s="8"/>
-      <c r="CO26" s="17"/>
-      <c r="CP26" s="20"/>
-      <c r="CQ26" s="20"/>
-      <c r="CR26" s="20"/>
-      <c r="CS26" s="20"/>
-      <c r="CT26" s="20"/>
-      <c r="CU26" s="21"/>
-      <c r="CX26" s="16"/>
+      <c r="CO26" s="16"/>
+      <c r="CP26" s="19"/>
+      <c r="CQ26" s="19"/>
+      <c r="CR26" s="19"/>
+      <c r="CS26" s="19"/>
+      <c r="CT26" s="19"/>
+      <c r="CU26" s="20"/>
+      <c r="CX26" s="15"/>
       <c r="CY26" s="3"/>
       <c r="CZ26" s="3"/>
       <c r="DA26" s="3"/>
       <c r="DB26" s="3"/>
       <c r="DC26" s="5"/>
     </row>
-    <row r="27" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
       <c r="I27" s="3"/>
@@ -3857,12 +3857,12 @@
       <c r="BC27" s="3"/>
       <c r="BD27" s="3"/>
       <c r="BE27" s="9"/>
-      <c r="BF27" s="15"/>
-      <c r="BG27" s="15"/>
-      <c r="BH27" s="15"/>
-      <c r="BI27" s="15"/>
-      <c r="BJ27" s="15"/>
-      <c r="BK27" s="15"/>
+      <c r="BF27" s="14"/>
+      <c r="BG27" s="14"/>
+      <c r="BH27" s="14"/>
+      <c r="BI27" s="14"/>
+      <c r="BJ27" s="14"/>
+      <c r="BK27" s="14"/>
       <c r="BL27" s="3"/>
       <c r="BM27" s="3"/>
       <c r="BN27" s="8"/>
@@ -3890,31 +3890,31 @@
       <c r="CJ27" s="8"/>
       <c r="CK27" s="3"/>
       <c r="CL27" s="3"/>
-      <c r="CM27" s="18"/>
+      <c r="CM27" s="17"/>
       <c r="CN27" s="8"/>
-      <c r="CO27" s="17"/>
-      <c r="CP27" s="20"/>
-      <c r="CQ27" s="20"/>
-      <c r="CR27" s="20"/>
-      <c r="CS27" s="20"/>
-      <c r="CT27" s="20"/>
-      <c r="CU27" s="21"/>
-      <c r="CX27" s="16"/>
+      <c r="CO27" s="16"/>
+      <c r="CP27" s="19"/>
+      <c r="CQ27" s="19"/>
+      <c r="CR27" s="19"/>
+      <c r="CS27" s="19"/>
+      <c r="CT27" s="19"/>
+      <c r="CU27" s="20"/>
+      <c r="CX27" s="15"/>
       <c r="CY27" s="3"/>
       <c r="CZ27" s="3"/>
       <c r="DA27" s="3"/>
       <c r="DB27" s="3"/>
       <c r="DC27" s="5"/>
     </row>
-    <row r="28" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
       <c r="I28" s="3"/>
@@ -3955,12 +3955,12 @@
       <c r="AR28" s="3"/>
       <c r="AS28" s="8"/>
       <c r="AT28" s="8"/>
-      <c r="AU28" s="15"/>
-      <c r="AV28" s="15"/>
-      <c r="AW28" s="15"/>
-      <c r="AX28" s="15"/>
-      <c r="AY28" s="15"/>
-      <c r="AZ28" s="15"/>
+      <c r="AU28" s="14"/>
+      <c r="AV28" s="14"/>
+      <c r="AW28" s="14"/>
+      <c r="AX28" s="14"/>
+      <c r="AY28" s="14"/>
+      <c r="AZ28" s="14"/>
       <c r="BA28" s="8"/>
       <c r="BB28" s="8"/>
       <c r="BC28" s="3"/>
@@ -3999,31 +3999,31 @@
       <c r="CJ28" s="8"/>
       <c r="CK28" s="3"/>
       <c r="CL28" s="3"/>
-      <c r="CM28" s="18"/>
+      <c r="CM28" s="17"/>
       <c r="CN28" s="8"/>
-      <c r="CO28" s="17"/>
-      <c r="CP28" s="20"/>
-      <c r="CQ28" s="20"/>
-      <c r="CR28" s="20"/>
-      <c r="CS28" s="20"/>
-      <c r="CT28" s="20"/>
-      <c r="CU28" s="21"/>
-      <c r="CX28" s="16"/>
+      <c r="CO28" s="16"/>
+      <c r="CP28" s="19"/>
+      <c r="CQ28" s="19"/>
+      <c r="CR28" s="19"/>
+      <c r="CS28" s="19"/>
+      <c r="CT28" s="19"/>
+      <c r="CU28" s="20"/>
+      <c r="CX28" s="15"/>
       <c r="CY28" s="3"/>
       <c r="CZ28" s="3"/>
       <c r="DA28" s="3"/>
       <c r="DB28" s="3"/>
       <c r="DC28" s="5"/>
     </row>
-    <row r="29" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
       <c r="I29" s="3"/>
@@ -4064,10 +4064,10 @@
       <c r="AR29" s="3"/>
       <c r="AS29" s="8"/>
       <c r="AT29" s="8"/>
-      <c r="AU29" s="15"/>
-      <c r="AV29" s="15"/>
-      <c r="AW29" s="15"/>
-      <c r="AX29" s="15"/>
+      <c r="AU29" s="14"/>
+      <c r="AV29" s="14"/>
+      <c r="AW29" s="14"/>
+      <c r="AX29" s="14"/>
       <c r="AY29" s="3"/>
       <c r="AZ29" s="3"/>
       <c r="BA29" s="8"/>
@@ -4108,31 +4108,31 @@
       <c r="CJ29" s="8"/>
       <c r="CK29" s="3"/>
       <c r="CL29" s="3"/>
-      <c r="CM29" s="18"/>
+      <c r="CM29" s="17"/>
       <c r="CN29" s="8"/>
-      <c r="CO29" s="17"/>
-      <c r="CP29" s="20"/>
-      <c r="CQ29" s="20"/>
-      <c r="CR29" s="20"/>
-      <c r="CS29" s="20"/>
-      <c r="CT29" s="20"/>
-      <c r="CU29" s="21"/>
-      <c r="CX29" s="16"/>
+      <c r="CO29" s="16"/>
+      <c r="CP29" s="19"/>
+      <c r="CQ29" s="19"/>
+      <c r="CR29" s="19"/>
+      <c r="CS29" s="19"/>
+      <c r="CT29" s="19"/>
+      <c r="CU29" s="20"/>
+      <c r="CX29" s="15"/>
       <c r="CY29" s="3"/>
       <c r="CZ29" s="3"/>
       <c r="DA29" s="3"/>
       <c r="DB29" s="3"/>
       <c r="DC29" s="5"/>
     </row>
-    <row r="30" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
       <c r="I30" s="3"/>
@@ -4177,8 +4177,8 @@
       <c r="AV30" s="3"/>
       <c r="AW30" s="8"/>
       <c r="AX30" s="8"/>
-      <c r="AY30" s="15"/>
-      <c r="AZ30" s="15"/>
+      <c r="AY30" s="14"/>
+      <c r="AZ30" s="14"/>
       <c r="BA30" s="8"/>
       <c r="BB30" s="8"/>
       <c r="BC30" s="3"/>
@@ -4217,31 +4217,31 @@
       <c r="CJ30" s="8"/>
       <c r="CK30" s="3"/>
       <c r="CL30" s="3"/>
-      <c r="CM30" s="18"/>
+      <c r="CM30" s="17"/>
       <c r="CN30" s="8"/>
-      <c r="CO30" s="17"/>
-      <c r="CP30" s="20"/>
-      <c r="CQ30" s="20"/>
-      <c r="CR30" s="20"/>
-      <c r="CS30" s="20"/>
-      <c r="CT30" s="20"/>
-      <c r="CU30" s="21"/>
-      <c r="CX30" s="16"/>
+      <c r="CO30" s="16"/>
+      <c r="CP30" s="19"/>
+      <c r="CQ30" s="19"/>
+      <c r="CR30" s="19"/>
+      <c r="CS30" s="19"/>
+      <c r="CT30" s="19"/>
+      <c r="CU30" s="20"/>
+      <c r="CX30" s="15"/>
       <c r="CY30" s="3"/>
       <c r="CZ30" s="3"/>
       <c r="DA30" s="3"/>
       <c r="DB30" s="3"/>
       <c r="DC30" s="5"/>
     </row>
-    <row r="31" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
       <c r="I31" s="3"/>
@@ -4288,10 +4288,10 @@
       <c r="AX31" s="8"/>
       <c r="AY31" s="3"/>
       <c r="AZ31" s="3"/>
-      <c r="BA31" s="15"/>
-      <c r="BB31" s="15"/>
-      <c r="BC31" s="15"/>
-      <c r="BD31" s="15"/>
+      <c r="BA31" s="14"/>
+      <c r="BB31" s="14"/>
+      <c r="BC31" s="14"/>
+      <c r="BD31" s="14"/>
       <c r="BE31" s="9"/>
       <c r="BF31" s="8"/>
       <c r="BG31" s="8"/>
@@ -4326,31 +4326,31 @@
       <c r="CJ31" s="8"/>
       <c r="CK31" s="3"/>
       <c r="CL31" s="3"/>
-      <c r="CM31" s="18"/>
+      <c r="CM31" s="17"/>
       <c r="CN31" s="8"/>
-      <c r="CO31" s="17"/>
-      <c r="CP31" s="20"/>
-      <c r="CQ31" s="20"/>
-      <c r="CR31" s="20"/>
-      <c r="CS31" s="20"/>
-      <c r="CT31" s="20"/>
-      <c r="CU31" s="21"/>
-      <c r="CX31" s="16"/>
+      <c r="CO31" s="16"/>
+      <c r="CP31" s="19"/>
+      <c r="CQ31" s="19"/>
+      <c r="CR31" s="19"/>
+      <c r="CS31" s="19"/>
+      <c r="CT31" s="19"/>
+      <c r="CU31" s="20"/>
+      <c r="CX31" s="15"/>
       <c r="CY31" s="3"/>
       <c r="CZ31" s="3"/>
       <c r="DA31" s="3"/>
       <c r="DB31" s="3"/>
       <c r="DC31" s="5"/>
     </row>
-    <row r="32" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="3"/>
@@ -4397,8 +4397,8 @@
       <c r="AX32" s="8"/>
       <c r="AY32" s="3"/>
       <c r="AZ32" s="3"/>
-      <c r="BA32" s="15"/>
-      <c r="BB32" s="15"/>
+      <c r="BA32" s="14"/>
+      <c r="BB32" s="14"/>
       <c r="BC32" s="3"/>
       <c r="BD32" s="3"/>
       <c r="BE32" s="9"/>
@@ -4435,31 +4435,31 @@
       <c r="CJ32" s="8"/>
       <c r="CK32" s="3"/>
       <c r="CL32" s="3"/>
-      <c r="CM32" s="18"/>
+      <c r="CM32" s="17"/>
       <c r="CN32" s="8"/>
-      <c r="CO32" s="17"/>
-      <c r="CP32" s="20"/>
-      <c r="CQ32" s="20"/>
-      <c r="CR32" s="20"/>
-      <c r="CS32" s="20"/>
-      <c r="CT32" s="20"/>
-      <c r="CU32" s="21"/>
-      <c r="CX32" s="16"/>
+      <c r="CO32" s="16"/>
+      <c r="CP32" s="19"/>
+      <c r="CQ32" s="19"/>
+      <c r="CR32" s="19"/>
+      <c r="CS32" s="19"/>
+      <c r="CT32" s="19"/>
+      <c r="CU32" s="20"/>
+      <c r="CX32" s="15"/>
       <c r="CY32" s="3"/>
       <c r="CZ32" s="3"/>
       <c r="DA32" s="3"/>
       <c r="DB32" s="3"/>
       <c r="DC32" s="5"/>
     </row>
-    <row r="33" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="18"/>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
       <c r="I33" s="3"/>
@@ -4506,8 +4506,8 @@
       <c r="AX33" s="8"/>
       <c r="AY33" s="3"/>
       <c r="AZ33" s="3"/>
-      <c r="BA33" s="15"/>
-      <c r="BB33" s="15"/>
+      <c r="BA33" s="14"/>
+      <c r="BB33" s="14"/>
       <c r="BC33" s="3"/>
       <c r="BD33" s="3"/>
       <c r="BE33" s="9"/>
@@ -4544,31 +4544,31 @@
       <c r="CJ33" s="8"/>
       <c r="CK33" s="3"/>
       <c r="CL33" s="3"/>
-      <c r="CM33" s="18"/>
+      <c r="CM33" s="17"/>
       <c r="CN33" s="8"/>
-      <c r="CO33" s="17"/>
-      <c r="CP33" s="20"/>
-      <c r="CQ33" s="20"/>
-      <c r="CR33" s="20"/>
-      <c r="CS33" s="20"/>
-      <c r="CT33" s="20"/>
-      <c r="CU33" s="21"/>
-      <c r="CX33" s="16"/>
+      <c r="CO33" s="16"/>
+      <c r="CP33" s="19"/>
+      <c r="CQ33" s="19"/>
+      <c r="CR33" s="19"/>
+      <c r="CS33" s="19"/>
+      <c r="CT33" s="19"/>
+      <c r="CU33" s="20"/>
+      <c r="CX33" s="15"/>
       <c r="CY33" s="3"/>
       <c r="CZ33" s="3"/>
       <c r="DA33" s="3"/>
       <c r="DB33" s="3"/>
       <c r="DC33" s="5"/>
     </row>
-    <row r="34" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
       <c r="I34" s="3"/>
@@ -4647,37 +4647,37 @@
       <c r="CD34" s="3"/>
       <c r="CE34" s="7"/>
       <c r="CF34" s="8"/>
-      <c r="CG34" s="15"/>
-      <c r="CH34" s="15"/>
+      <c r="CG34" s="14"/>
+      <c r="CH34" s="14"/>
       <c r="CI34" s="7"/>
       <c r="CJ34" s="8"/>
       <c r="CK34" s="3"/>
       <c r="CL34" s="3"/>
-      <c r="CM34" s="18"/>
+      <c r="CM34" s="17"/>
       <c r="CN34" s="8"/>
-      <c r="CO34" s="17"/>
-      <c r="CP34" s="20"/>
-      <c r="CQ34" s="20"/>
-      <c r="CR34" s="20"/>
-      <c r="CS34" s="20"/>
-      <c r="CT34" s="20"/>
-      <c r="CU34" s="21"/>
-      <c r="CX34" s="16"/>
+      <c r="CO34" s="16"/>
+      <c r="CP34" s="19"/>
+      <c r="CQ34" s="19"/>
+      <c r="CR34" s="19"/>
+      <c r="CS34" s="19"/>
+      <c r="CT34" s="19"/>
+      <c r="CU34" s="20"/>
+      <c r="CX34" s="15"/>
       <c r="CY34" s="3"/>
       <c r="CZ34" s="3"/>
       <c r="DA34" s="3"/>
       <c r="DB34" s="3"/>
       <c r="DC34" s="5"/>
     </row>
-    <row r="35" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
       <c r="I35" s="3"/>
@@ -4756,37 +4756,37 @@
       <c r="CD35" s="3"/>
       <c r="CE35" s="7"/>
       <c r="CF35" s="8"/>
-      <c r="CG35" s="15"/>
-      <c r="CH35" s="15"/>
+      <c r="CG35" s="14"/>
+      <c r="CH35" s="14"/>
       <c r="CI35" s="7"/>
       <c r="CJ35" s="8"/>
       <c r="CK35" s="3"/>
       <c r="CL35" s="3"/>
-      <c r="CM35" s="18"/>
+      <c r="CM35" s="17"/>
       <c r="CN35" s="8"/>
-      <c r="CO35" s="17"/>
-      <c r="CP35" s="20"/>
-      <c r="CQ35" s="20"/>
-      <c r="CR35" s="20"/>
-      <c r="CS35" s="20"/>
-      <c r="CT35" s="20"/>
-      <c r="CU35" s="21"/>
-      <c r="CX35" s="16"/>
+      <c r="CO35" s="16"/>
+      <c r="CP35" s="19"/>
+      <c r="CQ35" s="19"/>
+      <c r="CR35" s="19"/>
+      <c r="CS35" s="19"/>
+      <c r="CT35" s="19"/>
+      <c r="CU35" s="20"/>
+      <c r="CX35" s="15"/>
       <c r="CY35" s="3"/>
       <c r="CZ35" s="3"/>
       <c r="DA35" s="3"/>
       <c r="DB35" s="3"/>
       <c r="DC35" s="5"/>
     </row>
-    <row r="36" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
       <c r="I36" s="3"/>
@@ -4852,12 +4852,12 @@
       <c r="BQ36" s="3"/>
       <c r="BR36" s="8"/>
       <c r="BS36" s="7"/>
-      <c r="BT36" s="15"/>
-      <c r="BU36" s="15"/>
-      <c r="BV36" s="15"/>
-      <c r="BW36" s="15"/>
-      <c r="BX36" s="15"/>
-      <c r="BY36" s="15"/>
+      <c r="BT36" s="14"/>
+      <c r="BU36" s="14"/>
+      <c r="BV36" s="14"/>
+      <c r="BW36" s="14"/>
+      <c r="BX36" s="14"/>
+      <c r="BY36" s="14"/>
       <c r="BZ36" s="9"/>
       <c r="CA36" s="7"/>
       <c r="CB36" s="8"/>
@@ -4871,31 +4871,31 @@
       <c r="CJ36" s="8"/>
       <c r="CK36" s="3"/>
       <c r="CL36" s="3"/>
-      <c r="CM36" s="18"/>
+      <c r="CM36" s="17"/>
       <c r="CN36" s="8"/>
-      <c r="CO36" s="17"/>
-      <c r="CP36" s="20"/>
-      <c r="CQ36" s="20"/>
-      <c r="CR36" s="20"/>
-      <c r="CS36" s="20"/>
-      <c r="CT36" s="20"/>
-      <c r="CU36" s="21"/>
-      <c r="CX36" s="16"/>
+      <c r="CO36" s="16"/>
+      <c r="CP36" s="19"/>
+      <c r="CQ36" s="19"/>
+      <c r="CR36" s="19"/>
+      <c r="CS36" s="19"/>
+      <c r="CT36" s="19"/>
+      <c r="CU36" s="20"/>
+      <c r="CX36" s="15"/>
       <c r="CY36" s="3"/>
       <c r="CZ36" s="3"/>
       <c r="DA36" s="3"/>
       <c r="DB36" s="3"/>
       <c r="DC36" s="5"/>
     </row>
-    <row r="37" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
       <c r="I37" s="3"/>
@@ -4959,8 +4959,8 @@
       <c r="BO37" s="8"/>
       <c r="BP37" s="3"/>
       <c r="BQ37" s="3"/>
-      <c r="BR37" s="15"/>
-      <c r="BS37" s="15"/>
+      <c r="BR37" s="14"/>
+      <c r="BS37" s="14"/>
       <c r="BT37" s="3"/>
       <c r="BU37" s="3"/>
       <c r="BV37" s="8"/>
@@ -4980,31 +4980,31 @@
       <c r="CJ37" s="8"/>
       <c r="CK37" s="3"/>
       <c r="CL37" s="3"/>
-      <c r="CM37" s="18"/>
+      <c r="CM37" s="17"/>
       <c r="CN37" s="8"/>
-      <c r="CO37" s="17"/>
-      <c r="CP37" s="20"/>
-      <c r="CQ37" s="20"/>
-      <c r="CR37" s="20"/>
-      <c r="CS37" s="20"/>
-      <c r="CT37" s="20"/>
-      <c r="CU37" s="21"/>
-      <c r="CX37" s="16"/>
+      <c r="CO37" s="16"/>
+      <c r="CP37" s="19"/>
+      <c r="CQ37" s="19"/>
+      <c r="CR37" s="19"/>
+      <c r="CS37" s="19"/>
+      <c r="CT37" s="19"/>
+      <c r="CU37" s="20"/>
+      <c r="CX37" s="15"/>
       <c r="CY37" s="3"/>
       <c r="CZ37" s="3"/>
       <c r="DA37" s="3"/>
       <c r="DB37" s="3"/>
       <c r="DC37" s="5"/>
     </row>
-    <row r="38" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
       <c r="I38" s="3"/>
@@ -5074,8 +5074,8 @@
       <c r="BU38" s="3"/>
       <c r="BV38" s="8"/>
       <c r="BW38" s="7"/>
-      <c r="BX38" s="15"/>
-      <c r="BY38" s="15"/>
+      <c r="BX38" s="14"/>
+      <c r="BY38" s="14"/>
       <c r="BZ38" s="9"/>
       <c r="CA38" s="7"/>
       <c r="CB38" s="8"/>
@@ -5089,31 +5089,31 @@
       <c r="CJ38" s="8"/>
       <c r="CK38" s="3"/>
       <c r="CL38" s="3"/>
-      <c r="CM38" s="18"/>
+      <c r="CM38" s="17"/>
       <c r="CN38" s="8"/>
-      <c r="CO38" s="17"/>
-      <c r="CP38" s="20"/>
-      <c r="CQ38" s="20"/>
-      <c r="CR38" s="20"/>
-      <c r="CS38" s="20"/>
-      <c r="CT38" s="20"/>
-      <c r="CU38" s="21"/>
-      <c r="CX38" s="16"/>
+      <c r="CO38" s="16"/>
+      <c r="CP38" s="19"/>
+      <c r="CQ38" s="19"/>
+      <c r="CR38" s="19"/>
+      <c r="CS38" s="19"/>
+      <c r="CT38" s="19"/>
+      <c r="CU38" s="20"/>
+      <c r="CX38" s="15"/>
       <c r="CY38" s="3"/>
       <c r="CZ38" s="3"/>
       <c r="DA38" s="3"/>
       <c r="DB38" s="3"/>
       <c r="DC38" s="5"/>
     </row>
-    <row r="39" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
       <c r="I39" s="3"/>
@@ -5175,8 +5175,8 @@
       <c r="BM39" s="3"/>
       <c r="BN39" s="8"/>
       <c r="BO39" s="8"/>
-      <c r="BP39" s="15"/>
-      <c r="BQ39" s="15"/>
+      <c r="BP39" s="14"/>
+      <c r="BQ39" s="14"/>
       <c r="BR39" s="8"/>
       <c r="BS39" s="7"/>
       <c r="BT39" s="3"/>
@@ -5198,31 +5198,31 @@
       <c r="CJ39" s="8"/>
       <c r="CK39" s="3"/>
       <c r="CL39" s="3"/>
-      <c r="CM39" s="18"/>
+      <c r="CM39" s="17"/>
       <c r="CN39" s="8"/>
-      <c r="CO39" s="17"/>
-      <c r="CP39" s="20"/>
-      <c r="CQ39" s="20"/>
-      <c r="CR39" s="20"/>
-      <c r="CS39" s="20"/>
-      <c r="CT39" s="20"/>
-      <c r="CU39" s="21"/>
-      <c r="CX39" s="16"/>
+      <c r="CO39" s="16"/>
+      <c r="CP39" s="19"/>
+      <c r="CQ39" s="19"/>
+      <c r="CR39" s="19"/>
+      <c r="CS39" s="19"/>
+      <c r="CT39" s="19"/>
+      <c r="CU39" s="20"/>
+      <c r="CX39" s="15"/>
       <c r="CY39" s="3"/>
       <c r="CZ39" s="3"/>
       <c r="DA39" s="3"/>
       <c r="DB39" s="3"/>
       <c r="DC39" s="5"/>
     </row>
-    <row r="40" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
       <c r="I40" s="3"/>
@@ -5282,8 +5282,8 @@
       <c r="BK40" s="8"/>
       <c r="BL40" s="3"/>
       <c r="BM40" s="3"/>
-      <c r="BN40" s="15"/>
-      <c r="BO40" s="15"/>
+      <c r="BN40" s="14"/>
+      <c r="BO40" s="14"/>
       <c r="BP40" s="3"/>
       <c r="BQ40" s="3"/>
       <c r="BR40" s="8"/>
@@ -5307,31 +5307,31 @@
       <c r="CJ40" s="8"/>
       <c r="CK40" s="3"/>
       <c r="CL40" s="3"/>
-      <c r="CM40" s="18"/>
+      <c r="CM40" s="17"/>
       <c r="CN40" s="8"/>
-      <c r="CO40" s="17"/>
-      <c r="CP40" s="20"/>
-      <c r="CQ40" s="20"/>
-      <c r="CR40" s="20"/>
-      <c r="CS40" s="20"/>
-      <c r="CT40" s="20"/>
-      <c r="CU40" s="21"/>
-      <c r="CX40" s="16"/>
+      <c r="CO40" s="16"/>
+      <c r="CP40" s="19"/>
+      <c r="CQ40" s="19"/>
+      <c r="CR40" s="19"/>
+      <c r="CS40" s="19"/>
+      <c r="CT40" s="19"/>
+      <c r="CU40" s="20"/>
+      <c r="CX40" s="15"/>
       <c r="CY40" s="3"/>
       <c r="CZ40" s="3"/>
       <c r="DA40" s="3"/>
       <c r="DB40" s="3"/>
       <c r="DC40" s="5"/>
     </row>
-    <row r="41" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
       <c r="I41" s="3"/>
@@ -5416,31 +5416,31 @@
       <c r="CJ41" s="8"/>
       <c r="CK41" s="3"/>
       <c r="CL41" s="3"/>
-      <c r="CM41" s="18"/>
+      <c r="CM41" s="17"/>
       <c r="CN41" s="8"/>
-      <c r="CO41" s="17"/>
-      <c r="CP41" s="20"/>
-      <c r="CQ41" s="20"/>
-      <c r="CR41" s="20"/>
-      <c r="CS41" s="20"/>
-      <c r="CT41" s="20"/>
-      <c r="CU41" s="21"/>
-      <c r="CX41" s="16"/>
+      <c r="CO41" s="16"/>
+      <c r="CP41" s="19"/>
+      <c r="CQ41" s="19"/>
+      <c r="CR41" s="19"/>
+      <c r="CS41" s="19"/>
+      <c r="CT41" s="19"/>
+      <c r="CU41" s="20"/>
+      <c r="CX41" s="15"/>
       <c r="CY41" s="3"/>
       <c r="CZ41" s="3"/>
       <c r="DA41" s="3"/>
       <c r="DB41" s="3"/>
       <c r="DC41" s="5"/>
     </row>
-    <row r="42" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
       <c r="I42" s="3"/>
@@ -5513,10 +5513,10 @@
       <c r="BX42" s="3"/>
       <c r="BY42" s="3"/>
       <c r="BZ42" s="9"/>
-      <c r="CA42" s="15"/>
-      <c r="CB42" s="15"/>
-      <c r="CC42" s="15"/>
-      <c r="CD42" s="15"/>
+      <c r="CA42" s="14"/>
+      <c r="CB42" s="14"/>
+      <c r="CC42" s="14"/>
+      <c r="CD42" s="14"/>
       <c r="CE42" s="7"/>
       <c r="CF42" s="8"/>
       <c r="CG42" s="3"/>
@@ -5525,31 +5525,31 @@
       <c r="CJ42" s="8"/>
       <c r="CK42" s="3"/>
       <c r="CL42" s="3"/>
-      <c r="CM42" s="18"/>
+      <c r="CM42" s="17"/>
       <c r="CN42" s="8"/>
-      <c r="CO42" s="17"/>
-      <c r="CP42" s="20"/>
-      <c r="CQ42" s="20"/>
-      <c r="CR42" s="20"/>
-      <c r="CS42" s="20"/>
-      <c r="CT42" s="20"/>
-      <c r="CU42" s="21"/>
-      <c r="CX42" s="16"/>
+      <c r="CO42" s="16"/>
+      <c r="CP42" s="19"/>
+      <c r="CQ42" s="19"/>
+      <c r="CR42" s="19"/>
+      <c r="CS42" s="19"/>
+      <c r="CT42" s="19"/>
+      <c r="CU42" s="20"/>
+      <c r="CX42" s="15"/>
       <c r="CY42" s="3"/>
       <c r="CZ42" s="3"/>
       <c r="DA42" s="3"/>
       <c r="DB42" s="3"/>
       <c r="DC42" s="5"/>
     </row>
-    <row r="43" spans="1:107" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:107" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="19"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="3"/>
@@ -5622,10 +5622,10 @@
       <c r="BX43" s="3"/>
       <c r="BY43" s="3"/>
       <c r="BZ43" s="9"/>
-      <c r="CA43" s="15"/>
-      <c r="CB43" s="15"/>
-      <c r="CC43" s="15"/>
-      <c r="CD43" s="15"/>
+      <c r="CA43" s="14"/>
+      <c r="CB43" s="14"/>
+      <c r="CC43" s="14"/>
+      <c r="CD43" s="14"/>
       <c r="CE43" s="7"/>
       <c r="CF43" s="8"/>
       <c r="CG43" s="3"/>
@@ -5634,16 +5634,16 @@
       <c r="CJ43" s="8"/>
       <c r="CK43" s="3"/>
       <c r="CL43" s="3"/>
-      <c r="CM43" s="18"/>
+      <c r="CM43" s="17"/>
       <c r="CN43" s="8"/>
-      <c r="CO43" s="17"/>
-      <c r="CP43" s="20"/>
-      <c r="CQ43" s="20"/>
-      <c r="CR43" s="20"/>
-      <c r="CS43" s="20"/>
-      <c r="CT43" s="20"/>
-      <c r="CU43" s="21"/>
-      <c r="CX43" s="16"/>
+      <c r="CO43" s="16"/>
+      <c r="CP43" s="19"/>
+      <c r="CQ43" s="19"/>
+      <c r="CR43" s="19"/>
+      <c r="CS43" s="19"/>
+      <c r="CT43" s="19"/>
+      <c r="CU43" s="20"/>
+      <c r="CX43" s="15"/>
       <c r="CY43" s="3"/>
       <c r="CZ43" s="3"/>
       <c r="DA43" s="3"/>
@@ -5726,26 +5726,26 @@
       <c r="BX44" s="3"/>
       <c r="BY44" s="3"/>
       <c r="CB44" s="8"/>
-      <c r="CC44" s="15"/>
-      <c r="CD44" s="15"/>
-      <c r="CE44" s="15"/>
-      <c r="CF44" s="15"/>
+      <c r="CC44" s="14"/>
+      <c r="CD44" s="14"/>
+      <c r="CE44" s="14"/>
+      <c r="CF44" s="14"/>
       <c r="CG44" s="3"/>
       <c r="CH44" s="3"/>
       <c r="CJ44" s="8"/>
       <c r="CK44" s="3"/>
       <c r="CL44" s="3"/>
-      <c r="CM44" s="18"/>
+      <c r="CM44" s="17"/>
       <c r="CN44" s="8"/>
-      <c r="CO44" s="17"/>
-      <c r="CP44" s="20"/>
-      <c r="CQ44" s="20"/>
-      <c r="CR44" s="20"/>
-      <c r="CS44" s="20"/>
-      <c r="CT44" s="20"/>
+      <c r="CO44" s="16"/>
+      <c r="CP44" s="19"/>
+      <c r="CQ44" s="19"/>
+      <c r="CR44" s="19"/>
+      <c r="CS44" s="19"/>
+      <c r="CT44" s="19"/>
       <c r="CV44" s="3"/>
       <c r="CW44" s="3"/>
-      <c r="CX44" s="16"/>
+      <c r="CX44" s="15"/>
       <c r="CY44" s="3"/>
       <c r="CZ44" s="3"/>
       <c r="DA44" s="3"/>
@@ -5853,7 +5853,7 @@
       <c r="CU45" s="3"/>
       <c r="CV45" s="3"/>
       <c r="CW45" s="3"/>
-      <c r="CX45" s="16"/>
+      <c r="CX45" s="15"/>
       <c r="CY45" s="3"/>
       <c r="CZ45" s="3"/>
       <c r="DA45" s="3"/>

</xml_diff>